<commit_message>
add Koppen climate colors
</commit_message>
<xml_diff>
--- a/data/layouts/symbology.xlsx
+++ b/data/layouts/symbology.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rprojects\eamena-arches-dev\data\layouts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0786921D-A3EF-43DB-BF3D-8267D5023EEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D499DB77-D641-4980-99C7-59EABEAF76BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FBCDE9FA-39BE-454A-99C4-DA94C2CE115D}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FBCDE9FA-39BE-454A-99C4-DA94C2CE115D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="71">
   <si>
     <t>No Visible/Known</t>
   </si>
@@ -87,6 +87,168 @@
   </si>
   <si>
     <t>color</t>
+  </si>
+  <si>
+    <t>Af Tropical, rainforest</t>
+  </si>
+  <si>
+    <t>0000FF</t>
+  </si>
+  <si>
+    <t>Am Tropical, monsoon</t>
+  </si>
+  <si>
+    <t>0078FF</t>
+  </si>
+  <si>
+    <t>Aw Tropical, savannah</t>
+  </si>
+  <si>
+    <t>46AAF</t>
+  </si>
+  <si>
+    <t>BWh Arid, desert, hot</t>
+  </si>
+  <si>
+    <t>FF0000</t>
+  </si>
+  <si>
+    <t>BWk Arid, desert, cold</t>
+  </si>
+  <si>
+    <t>FF9696</t>
+  </si>
+  <si>
+    <t>BSh Arid, steppe, hot</t>
+  </si>
+  <si>
+    <t>F5A500</t>
+  </si>
+  <si>
+    <t>BSk Arid, steppe, cold</t>
+  </si>
+  <si>
+    <t>FFDC64</t>
+  </si>
+  <si>
+    <t>Csa Temperate, dry summer, hot summer</t>
+  </si>
+  <si>
+    <t>FFFF00</t>
+  </si>
+  <si>
+    <t>Csb Temperate, dry summer, warm summer</t>
+  </si>
+  <si>
+    <t>C8C800</t>
+  </si>
+  <si>
+    <t>Csc Temperate, dry summer, cold summer</t>
+  </si>
+  <si>
+    <t>Cwa Temperate, dry winter, hot summer</t>
+  </si>
+  <si>
+    <t>96FF96</t>
+  </si>
+  <si>
+    <t>Cwb Temperate, dry winter, warm summer</t>
+  </si>
+  <si>
+    <t>64C864</t>
+  </si>
+  <si>
+    <t>Cwc Temperate, dry winter, cold summer</t>
+  </si>
+  <si>
+    <t>Cfa Temperate, no dry season, hot summer</t>
+  </si>
+  <si>
+    <t>C8FF50</t>
+  </si>
+  <si>
+    <t>Cfb Temperate, no dry season, warm summer</t>
+  </si>
+  <si>
+    <t>64FF50</t>
+  </si>
+  <si>
+    <t>Cfc Temperate, no dry season, cold summer</t>
+  </si>
+  <si>
+    <t>32C800</t>
+  </si>
+  <si>
+    <t>Dsa Cold, dry summer, hot summer</t>
+  </si>
+  <si>
+    <t>FF00FF</t>
+  </si>
+  <si>
+    <t>Dsb Cold, dry summer, warm summer</t>
+  </si>
+  <si>
+    <t>C800C8</t>
+  </si>
+  <si>
+    <t>Dsc Cold, dry summer, cold summer</t>
+  </si>
+  <si>
+    <t>Dsd Cold, dry summer, very cold winter</t>
+  </si>
+  <si>
+    <t>Dwa Cold, dry winter, hot summer</t>
+  </si>
+  <si>
+    <t>AAAF</t>
+  </si>
+  <si>
+    <t>Dwb Cold, dry winter, warm summer</t>
+  </si>
+  <si>
+    <t>5A78DC</t>
+  </si>
+  <si>
+    <t>Dwc Cold, dry winter, cold summer</t>
+  </si>
+  <si>
+    <t>4B50B4</t>
+  </si>
+  <si>
+    <t>Dwd Cold, dry winter, very cold winter</t>
+  </si>
+  <si>
+    <t>Dfa Cold, no dry season, hot summer</t>
+  </si>
+  <si>
+    <t>00FFFF</t>
+  </si>
+  <si>
+    <t>Dfb Cold, no dry season, warm summer</t>
+  </si>
+  <si>
+    <t>37C8FF</t>
+  </si>
+  <si>
+    <t>Dfc Cold, no dry season, cold summer</t>
+  </si>
+  <si>
+    <t>007D7D</t>
+  </si>
+  <si>
+    <t>Dfd Cold, no dry season, very cold winter</t>
+  </si>
+  <si>
+    <t>00465F</t>
+  </si>
+  <si>
+    <t>ET Polar, tundra</t>
+  </si>
+  <si>
+    <t>B2B2B2</t>
+  </si>
+  <si>
+    <t>EF Polar, frost</t>
   </si>
 </sst>
 </file>
@@ -598,16 +760,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C624EBA0-A399-46E8-A080-116D9313C5AC}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="55.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="8.88671875" style="1"/>
@@ -653,7 +815,7 @@
         <v>11</v>
       </c>
       <c r="D3" s="1" t="str">
-        <f t="shared" ref="D3:D8" si="0">CONCATENATE("![#",C3,"](https://placehold.co/15x15/",C3,"/",C3,".png)")</f>
+        <f t="shared" ref="D3:D38" si="0">CONCATENATE("![#",C3,"](https://placehold.co/15x15/",C3,"/",C3,".png)")</f>
         <v>![#FECC5C](https://placehold.co/15x15/FECC5C/FECC5C.png)</v>
       </c>
     </row>
@@ -730,6 +892,456 @@
       <c r="D8" s="1" t="str">
         <f t="shared" si="0"/>
         <v>![#808080](https://placehold.co/15x15/808080/808080.png)</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>1</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>![#0000FF](https://placehold.co/15x15/0000FF/0000FF.png)</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>2</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>![#0078FF](https://placehold.co/15x15/0078FF/0078FF.png)</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>3</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>![#46AAF](https://placehold.co/15x15/46AAF/46AAF.png)</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>4</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>![#FF0000](https://placehold.co/15x15/FF0000/FF0000.png)</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>5</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>![#FF9696](https://placehold.co/15x15/FF9696/FF9696.png)</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>6</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>![#F5A500](https://placehold.co/15x15/F5A500/F5A500.png)</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>7</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>![#FFDC64](https://placehold.co/15x15/FFDC64/FFDC64.png)</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>8</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>![#FFFF00](https://placehold.co/15x15/FFFF00/FFFF00.png)</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>9</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>![#C8C800](https://placehold.co/15x15/C8C800/C8C800.png)</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>10</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="1">
+        <v>969600</v>
+      </c>
+      <c r="D18" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>![#969600](https://placehold.co/15x15/969600/969600.png)</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>11</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>![#96FF96](https://placehold.co/15x15/96FF96/96FF96.png)</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>12</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>![#64C864](https://placehold.co/15x15/64C864/64C864.png)</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>13</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="1">
+        <v>329632</v>
+      </c>
+      <c r="D21" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>![#329632](https://placehold.co/15x15/329632/329632.png)</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>14</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>![#C8FF50](https://placehold.co/15x15/C8FF50/C8FF50.png)</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>15</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>![#64FF50](https://placehold.co/15x15/64FF50/64FF50.png)</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>16</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>![#32C800](https://placehold.co/15x15/32C800/32C800.png)</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>17</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D25" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>![#FF00FF](https://placehold.co/15x15/FF00FF/FF00FF.png)</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>18</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D26" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>![#C800C8](https://placehold.co/15x15/C800C8/C800C8.png)</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>19</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="1">
+        <v>963296</v>
+      </c>
+      <c r="D27" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>![#963296](https://placehold.co/15x15/963296/963296.png)</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>20</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" s="1">
+        <v>966496</v>
+      </c>
+      <c r="D28" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>![#966496](https://placehold.co/15x15/966496/966496.png)</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>21</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D29" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>![#AAAF](https://placehold.co/15x15/AAAF/AAAF.png)</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>22</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D30" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>![#5A78DC](https://placehold.co/15x15/5A78DC/5A78DC.png)</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>23</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D31" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>![#4B50B4](https://placehold.co/15x15/4B50B4/4B50B4.png)</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>24</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C32" s="1">
+        <v>320087</v>
+      </c>
+      <c r="D32" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>![#320087](https://placehold.co/15x15/320087/320087.png)</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>25</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D33" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>![#00FFFF](https://placehold.co/15x15/00FFFF/00FFFF.png)</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>26</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D34" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>![#37C8FF](https://placehold.co/15x15/37C8FF/37C8FF.png)</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>27</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D35" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>![#007D7D](https://placehold.co/15x15/007D7D/007D7D.png)</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>28</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D36" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>![#00465F](https://placehold.co/15x15/00465F/00465F.png)</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>29</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D37" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>![#B2B2B2](https://placehold.co/15x15/B2B2B2/B2B2B2.png)</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>30</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C38" s="1">
+        <v>666666</v>
+      </c>
+      <c r="D38" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>![#666666](https://placehold.co/15x15/666666/666666.png)</v>
       </c>
     </row>
   </sheetData>

</xml_diff>